<commit_message>
Implement backup & restore features
</commit_message>
<xml_diff>
--- a/src/main/resources/static/data/excel/SystemDataInit.xlsx
+++ b/src/main/resources/static/data/excel/SystemDataInit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App\FW_PMS\src\main\resources\static\data\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viet0\Projects\FW_PMS\src\main\resources\static\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B79E4C7-BE71-4C8A-BE97-0C6DDBB6ECE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8240796E-C090-4F5C-A6E3-EE8DD1CE8021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26340" yWindow="5220" windowWidth="24645" windowHeight="9075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BRANCH" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="ACCOUNT" sheetId="3" r:id="rId3"/>
     <sheet name="CUSTOMER" sheetId="4" r:id="rId4"/>
     <sheet name="SCHEDULE" sheetId="5" r:id="rId5"/>
+    <sheet name="SERIAL" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>BRANCH_CODE</t>
   </si>
@@ -137,6 +138,21 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>PREFIX</t>
+  </si>
+  <si>
+    <t>INIT_VALUE</t>
+  </si>
+  <si>
+    <t>CURRENT_VALUE</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>0000001</t>
   </si>
 </sst>
 </file>
@@ -172,8 +188,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,17 +473,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,7 +491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -495,13 +512,13 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -509,7 +526,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -517,7 +534,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -538,16 +555,16 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -573,7 +590,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -609,16 +626,16 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -629,7 +646,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -653,13 +670,13 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -670,7 +687,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -681,7 +698,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -692,7 +709,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -701,6 +718,43 @@
       </c>
       <c r="C4" t="s">
         <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC818D7-4632-45A7-9CD4-A0A10003E6AC}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>